<commit_message>
Added more CPU opcodes
</commit_message>
<xml_diff>
--- a/FinishedOpcodes.xlsx
+++ b/FinishedOpcodes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="26115" windowHeight="11055"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="26115" windowHeight="11055"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -553,9 +553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -755,12 +753,12 @@
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="2" t="s">
         <v>40</v>
       </c>
     </row>
@@ -780,12 +778,12 @@
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+      <c r="A45" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="2" t="s">
         <v>45</v>
       </c>
     </row>
@@ -810,22 +808,22 @@
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+      <c r="A51" s="2" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+      <c r="A52" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+      <c r="A53" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+      <c r="A54" s="2" t="s">
         <v>53</v>
       </c>
     </row>
@@ -835,7 +833,7 @@
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+      <c r="A56" s="2" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>

<commit_message>
All CPU opcodes added
Finished adding CPU opcodes. Haven't gotten to test all of them, so there are likely some bugs (particularly in ADC and SBC; not sure if I implemented the Overflow flag correctly in those operations).

Next step is figuring out how to implement the PPU and APU and get them to interact with the memory and CPU.
</commit_message>
<xml_diff>
--- a/FinishedOpcodes.xlsx
+++ b/FinishedOpcodes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="26115" windowHeight="11055"/>
+    <workbookView xWindow="0" yWindow="1350" windowWidth="26115" windowHeight="11055"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -233,9 +233,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -553,7 +552,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -603,12 +604,12 @@
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -623,22 +624,22 @@
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -683,12 +684,12 @@
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
     </row>
@@ -698,22 +699,22 @@
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
     </row>
@@ -723,7 +724,7 @@
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
     </row>
@@ -733,32 +734,32 @@
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
     </row>
@@ -768,7 +769,7 @@
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -778,62 +779,62 @@
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
+      <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+      <c r="A50" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
+      <c r="A52" s="1" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
+      <c r="A53" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
+      <c r="A54" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
+      <c r="A55" s="1" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
+      <c r="A56" s="1" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>